<commit_message>
add current price and TWII and TWOII and OTC option
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,80 +436,85 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>現價</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>日主力</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>周外資</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>72分上</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>72分下</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>月線</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>季線</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>年線</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>量MA5&gt;20</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>連3日&gt;MA5</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>daily_MACD</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>daily_RSI14</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>weekly_MACD</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>weekly_RSI14</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>趨勢</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>正加總</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>負加總</t>
         </is>
@@ -518,159 +523,225 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>0056.TW</t>
+          <t>TWII</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5,651</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>4,990</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>36.05</v>
-      </c>
-      <c r="E2" t="n">
-        <v>31.28</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>35.10-</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>34.38-</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>28.83-</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>- (13501919.75)</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0.19</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>57.23</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>1.83</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>78.04</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>++-----++++</t>
-        </is>
-      </c>
-      <c r="P2" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>5</v>
-      </c>
+          <t>18,096.07</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>00701.TW</t>
+          <t>TWOII</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>27.08</v>
-      </c>
-      <c r="E3" t="n">
-        <v>24.68</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>26.06+</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>25.84-</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>23.48-</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>- (318187.00)</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+          <t>238.67</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2427.TW</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>23.00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-220</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-125</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>24.30+</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>25.82+</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>23.13+</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>- (887668.60)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>-0.04</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>42.21</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0.78</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>65.10</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>+++-----+++</t>
-        </is>
-      </c>
-      <c r="P3" t="n">
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>-0.58</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>25.00</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.63</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>20.71</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>+--+++---+++</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>7</v>
+      </c>
+      <c r="R4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>1264.TWO</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>295.00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>294.5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>289</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>294.77-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>292.52-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>285.47-</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>- (820.05)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.66</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>37.50</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>76.00</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>+------+++++</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
         <v>6</v>
       </c>
-      <c r="Q3" t="n">
-        <v>5</v>
+      <c r="R5" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix input can't put char problem
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18,096.07</t>
+          <t>18,635.80</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -556,7 +556,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>238.67</t>
+          <t>245.11</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -579,48 +579,48 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>6435.TWO</t>
+          <t>00724B.TWO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>111.50</t>
+          <t>33.86</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>-122</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>-150</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>118.5</v>
+        <v>34.86</v>
       </c>
       <c r="F4" t="n">
-        <v>103</v>
+        <v>31.87</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>107.35-</t>
+          <t>34.36+</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>108.07-</t>
+          <t>33.92+</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>97.66+</t>
+          <t>33.07-</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>+ (23099.85)</t>
+          <t>+ (434037.95)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -630,286 +630,34 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0.23</t>
+          <t>0.09</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>61.29</t>
+          <t>45.66</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>3.53</t>
+          <t>0.36</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>64.98</t>
+          <t>61.11</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>+++--+--++++</t>
+          <t>+--++---++++</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>6770.TW</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>26.80</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-1,164</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-1,396</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>30.65</v>
-      </c>
-      <c r="F5" t="n">
-        <v>27.25</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>27.87+</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>28.80+</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>29.76+</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>- (717690.75)</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>-0.44</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>28.00</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>-0.36</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>42.15</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>+--+++---+-+</t>
-        </is>
-      </c>
-      <c r="Q5" t="n">
-        <v>6</v>
-      </c>
-      <c r="R5" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>3033.TW</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>31.00</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1,041</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1,129</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>31.45</v>
-      </c>
-      <c r="F6" t="n">
-        <v>28.05</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>30.37-</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>29.05-</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>29.89-</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>+ (2426811.30)</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>0.54</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>55.45</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>-0.09</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>83.96</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>+++-----++-+</t>
-        </is>
-      </c>
-      <c r="Q6" t="n">
-        <v>6</v>
-      </c>
-      <c r="R6" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>5410.TWO</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>33.40</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-5</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>-6</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>34.7</v>
-      </c>
-      <c r="F7" t="n">
-        <v>32.75</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>33.34-</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>33.20-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>33.81+</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>- (35305.05)</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>50.98</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>-0.00</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>55.43</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>+----+--++-+</t>
-        </is>
-      </c>
-      <c r="Q7" t="n">
         <v>5</v>
-      </c>
-      <c r="R7" t="n">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>